<commit_message>
added back to main menu btns and exit btns
</commit_message>
<xml_diff>
--- a/LoginPage/bin/Debug/net7.0-windows/Data/birds.xlsx
+++ b/LoginPage/bin/Debug/net7.0-windows/Data/birds.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ffgtf\Source\Repos\Bird-Project-For-College\LoginPage\bin\Debug\net7.0-windows\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tomer\source\repos\Bird-Project-For-College\LoginPage\bin\Debug\net7.0-windows\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE4AD682-68BB-4196-B517-5465F2446D53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23F4C9BA-2C83-4755-8104-C14A8528C6CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28410" yWindow="2130" windowWidth="27240" windowHeight="15495" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="44">
   <si>
     <t>bdika11</t>
   </si>
@@ -144,6 +144,21 @@
   </si>
   <si>
     <t>South America</t>
+  </si>
+  <si>
+    <t>tomer99</t>
+  </si>
+  <si>
+    <t>Tomer99!</t>
+  </si>
+  <si>
+    <t>Tomer91</t>
+  </si>
+  <si>
+    <t>Tomer9!!</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -462,10 +477,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView rightToLeft="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -501,6 +516,44 @@
       </c>
       <c r="C3">
         <v>123</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5">
+        <v>1121</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C7">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -512,7 +565,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54D0F034-6ABF-4A1B-831B-4EE238759774}">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
+    <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added cage link to birds
</commit_message>
<xml_diff>
--- a/LoginPage/bin/Debug/net7.0-windows/Data/birds.xlsx
+++ b/LoginPage/bin/Debug/net7.0-windows/Data/birds.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tomer\source\repos\Bird-Project-For-College\LoginPage\bin\Debug\net7.0-windows\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tomer\Source\Repos\Bird-Project-For-College\LoginPage\bin\Debug\net7.0-windows\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23F4C9BA-2C83-4755-8104-C14A8528C6CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C65AB91A-2763-4473-92A1-4054EEDAF9C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="55">
   <si>
     <t>bdika11</t>
   </si>
@@ -158,7 +158,40 @@
     <t>Tomer9!!</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
+    <t>ש</t>
+  </si>
+  <si>
+    <t>kakape98</t>
+  </si>
+  <si>
+    <t>kaka1998!</t>
+  </si>
+  <si>
+    <t>avivaa98</t>
+  </si>
+  <si>
+    <t>avivaa98!</t>
+  </si>
+  <si>
+    <t>a9</t>
+  </si>
+  <si>
+    <t>aaaaaa11</t>
+  </si>
+  <si>
+    <t>aaaaaa1!</t>
+  </si>
+  <si>
+    <t>a10</t>
+  </si>
+  <si>
+    <t>bbbbbb9</t>
+  </si>
+  <si>
+    <t>bbbbbb1!</t>
+  </si>
+  <si>
+    <t>Central America</t>
   </si>
 </sst>
 </file>
@@ -477,7 +510,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -552,8 +585,47 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" t="s">
+        <v>45</v>
+      </c>
       <c r="C7">
-        <v>3</v>
+        <v>334</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10">
+        <v>1113</v>
       </c>
     </row>
   </sheetData>
@@ -563,7 +635,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54D0F034-6ABF-4A1B-831B-4EE238759774}">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -720,6 +792,75 @@
         <v>1</v>
       </c>
     </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G7" s="1">
+        <v>45049</v>
+      </c>
+      <c r="H7" t="s">
+        <v>32</v>
+      </c>
+      <c r="I7">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G8" s="1">
+        <v>45049</v>
+      </c>
+      <c r="H8" t="s">
+        <v>32</v>
+      </c>
+      <c r="I8">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" t="s">
+        <v>54</v>
+      </c>
+      <c r="D9" t="s">
+        <v>37</v>
+      </c>
+      <c r="G9" s="1">
+        <v>45049</v>
+      </c>
+      <c r="H9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -727,7 +868,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38953711-B99E-424A-A94F-86EB399A85F5}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -871,6 +1012,40 @@
         <v>20</v>
       </c>
     </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9">
+        <v>6</v>
+      </c>
+      <c r="C9">
+        <v>6</v>
+      </c>
+      <c r="D9">
+        <v>6</v>
+      </c>
+      <c r="E9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <v>9</v>
+      </c>
+      <c r="D10">
+        <v>9</v>
+      </c>
+      <c r="E10" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fix bug with invalid input for bird id
</commit_message>
<xml_diff>
--- a/LoginPage/bin/Debug/net7.0-windows/Data/birds.xlsx
+++ b/LoginPage/bin/Debug/net7.0-windows/Data/birds.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tomer\source\repos\Bird-Project-For-College\LoginPage\bin\Debug\net7.0-windows\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF3F151E-325A-42AC-A415-B3CB5ECE7142}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E2E057A-856B-4206-939B-B6E68107CC5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="55">
   <si>
     <t>bdika11</t>
   </si>
@@ -635,7 +635,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54D0F034-6ABF-4A1B-831B-4EE238759774}">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -916,6 +916,32 @@
         <v>21</v>
       </c>
       <c r="I11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12">
+        <v>10</v>
+      </c>
+      <c r="G12" s="1">
+        <v>45049</v>
+      </c>
+      <c r="H12" t="s">
+        <v>21</v>
+      </c>
+      <c r="I12">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
upadte mom and dad check
</commit_message>
<xml_diff>
--- a/LoginPage/bin/Debug/net7.0-windows/Data/birds.xlsx
+++ b/LoginPage/bin/Debug/net7.0-windows/Data/birds.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tomer\source\repos\Bird-Project-For-College\LoginPage\bin\Debug\net7.0-windows\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hodaya Amiel\Source\Repos\Bird-Project-For-College\LoginPage\bin\Debug\net7.0-windows\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65E13335-E64E-46ED-B68A-6FAC5E4F0C60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5622D6AF-F55D-464A-AEE0-B5A54FBAFBC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1100" yWindow="1100" windowWidth="14400" windowHeight="7270" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="65">
   <si>
     <t>bdika11</t>
   </si>
@@ -216,6 +216,12 @@
   </si>
   <si>
     <t>daniel11!</t>
+  </si>
+  <si>
+    <t>daniel34</t>
+  </si>
+  <si>
+    <t>Daniel34!</t>
   </si>
 </sst>
 </file>
@@ -534,15 +540,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -553,7 +559,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -564,7 +570,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -575,7 +581,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>39</v>
       </c>
@@ -586,7 +592,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>41</v>
       </c>
@@ -597,7 +603,7 @@
         <v>1121</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>43</v>
       </c>
@@ -608,7 +614,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>44</v>
       </c>
@@ -619,7 +625,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>46</v>
       </c>
@@ -630,7 +636,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>49</v>
       </c>
@@ -641,7 +647,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>52</v>
       </c>
@@ -652,7 +658,7 @@
         <v>1113</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>55</v>
       </c>
@@ -663,7 +669,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>57</v>
       </c>
@@ -674,7 +680,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>59</v>
       </c>
@@ -685,7 +691,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>61</v>
       </c>
@@ -694,6 +700,17 @@
       </c>
       <c r="C14">
         <v>555</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15" t="s">
+        <v>64</v>
+      </c>
+      <c r="C15">
+        <v>777</v>
       </c>
     </row>
   </sheetData>
@@ -703,20 +720,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54D0F034-6ABF-4A1B-831B-4EE238759774}">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.5" customWidth="1"/>
-    <col min="3" max="3" width="12.625" customWidth="1"/>
+    <col min="3" max="3" width="12.58203125" customWidth="1"/>
     <col min="7" max="7" width="25.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -745,7 +762,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -768,7 +785,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -791,7 +808,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -814,7 +831,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -837,7 +854,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -860,7 +877,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -883,7 +900,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -906,7 +923,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -929,7 +946,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -958,7 +975,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -987,7 +1004,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1011,6 +1028,58 @@
       </c>
       <c r="I12">
         <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" t="s">
+        <v>54</v>
+      </c>
+      <c r="D13" t="s">
+        <v>37</v>
+      </c>
+      <c r="G13" s="1">
+        <v>45050</v>
+      </c>
+      <c r="H13" t="s">
+        <v>21</v>
+      </c>
+      <c r="I13">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" t="s">
+        <v>54</v>
+      </c>
+      <c r="D14" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14">
+        <v>7</v>
+      </c>
+      <c r="F14">
+        <v>12</v>
+      </c>
+      <c r="G14" s="1">
+        <v>45050</v>
+      </c>
+      <c r="H14" t="s">
+        <v>21</v>
+      </c>
+      <c r="I14">
+        <v>777</v>
       </c>
     </row>
   </sheetData>
@@ -1026,9 +1095,9 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -1045,7 +1114,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -1062,7 +1131,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -1079,7 +1148,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -1096,7 +1165,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -1113,7 +1182,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -1130,7 +1199,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -1147,7 +1216,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -1164,7 +1233,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>48</v>
       </c>
@@ -1181,7 +1250,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>51</v>
       </c>

</xml_diff>

<commit_message>
update Chick color generate function
</commit_message>
<xml_diff>
--- a/LoginPage/bin/Debug/net7.0-windows/Data/birds.xlsx
+++ b/LoginPage/bin/Debug/net7.0-windows/Data/birds.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aviv1\Documents\Bird-Project-For-College\LoginPage\bin\Debug\net7.0-windows\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{634A88CB-6C35-4FC6-8084-E9A234017A7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B770C168-A06A-4305-91EC-7E9BAE642C05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11295" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="73">
   <si>
     <t>bdika11</t>
   </si>
@@ -571,6 +571,11 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.625" customWidth="1"/>
+    <col min="2" max="2" width="13.75" customWidth="1"/>
+    <col min="3" max="3" width="11.25" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -757,8 +762,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54D0F034-6ABF-4A1B-831B-4EE238759774}">
   <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView rightToLeft="1" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -834,6 +839,15 @@
       <c r="I2">
         <v>1</v>
       </c>
+      <c r="J2" t="s">
+        <v>65</v>
+      </c>
+      <c r="K2" t="s">
+        <v>66</v>
+      </c>
+      <c r="L2" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3">
@@ -857,6 +871,15 @@
       <c r="I3">
         <v>1</v>
       </c>
+      <c r="J3" t="s">
+        <v>65</v>
+      </c>
+      <c r="K3" t="s">
+        <v>66</v>
+      </c>
+      <c r="L3" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4">
@@ -880,6 +903,15 @@
       <c r="I4">
         <v>1</v>
       </c>
+      <c r="J4" t="s">
+        <v>65</v>
+      </c>
+      <c r="K4" t="s">
+        <v>66</v>
+      </c>
+      <c r="L4" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5">
@@ -903,6 +935,15 @@
       <c r="I5">
         <v>1</v>
       </c>
+      <c r="J5" t="s">
+        <v>65</v>
+      </c>
+      <c r="K5" t="s">
+        <v>66</v>
+      </c>
+      <c r="L5" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6">
@@ -926,6 +967,15 @@
       <c r="I6">
         <v>1</v>
       </c>
+      <c r="J6" t="s">
+        <v>65</v>
+      </c>
+      <c r="K6" t="s">
+        <v>66</v>
+      </c>
+      <c r="L6" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7">
@@ -949,6 +999,15 @@
       <c r="I7">
         <v>106</v>
       </c>
+      <c r="J7" t="s">
+        <v>65</v>
+      </c>
+      <c r="K7" t="s">
+        <v>66</v>
+      </c>
+      <c r="L7" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8">
@@ -972,6 +1031,15 @@
       <c r="I8">
         <v>102</v>
       </c>
+      <c r="J8" t="s">
+        <v>65</v>
+      </c>
+      <c r="K8" t="s">
+        <v>66</v>
+      </c>
+      <c r="L8" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9">
@@ -995,6 +1063,15 @@
       <c r="I9">
         <v>1</v>
       </c>
+      <c r="J9" t="s">
+        <v>65</v>
+      </c>
+      <c r="K9" t="s">
+        <v>66</v>
+      </c>
+      <c r="L9" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10">
@@ -1024,6 +1101,15 @@
       <c r="I10">
         <v>1</v>
       </c>
+      <c r="J10" t="s">
+        <v>65</v>
+      </c>
+      <c r="K10" t="s">
+        <v>66</v>
+      </c>
+      <c r="L10" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11">
@@ -1053,6 +1139,15 @@
       <c r="I11">
         <v>1</v>
       </c>
+      <c r="J11" t="s">
+        <v>65</v>
+      </c>
+      <c r="K11" t="s">
+        <v>66</v>
+      </c>
+      <c r="L11" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12">
@@ -1079,6 +1174,15 @@
       <c r="I12">
         <v>1</v>
       </c>
+      <c r="J12" t="s">
+        <v>65</v>
+      </c>
+      <c r="K12" t="s">
+        <v>66</v>
+      </c>
+      <c r="L12" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13">
@@ -1102,6 +1206,15 @@
       <c r="I13">
         <v>777</v>
       </c>
+      <c r="J13" t="s">
+        <v>65</v>
+      </c>
+      <c r="K13" t="s">
+        <v>66</v>
+      </c>
+      <c r="L13" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14">
@@ -1130,6 +1243,15 @@
       </c>
       <c r="I14">
         <v>777</v>
+      </c>
+      <c r="J14" t="s">
+        <v>65</v>
+      </c>
+      <c r="K14" t="s">
+        <v>66</v>
+      </c>
+      <c r="L14" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
@@ -1173,7 +1295,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38953711-B99E-424A-A94F-86EB399A85F5}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView rightToLeft="1" workbookViewId="0">
+    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fixed double click cage, fixed cage adding input check
</commit_message>
<xml_diff>
--- a/LoginPage/bin/Debug/net7.0-windows/Data/birds.xlsx
+++ b/LoginPage/bin/Debug/net7.0-windows/Data/birds.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aviv1\Documents\Bird-Project-For-College\LoginPage\bin\Debug\net7.0-windows\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ffgtf\Source\Repos\Bird-Project-For-College1\LoginPage\bin\Debug\net7.0-windows\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BABC6BD-E7D8-4D8A-B4A0-C240B4EBF2DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8466F97-BA8B-4CD9-B3F2-2C3F080DA23C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28410" yWindow="2130" windowWidth="27240" windowHeight="15495" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="80">
   <si>
     <t>bdika11</t>
   </si>
@@ -125,9 +125,6 @@
     <t>Female</t>
   </si>
   <si>
-    <t>a1</t>
-  </si>
-  <si>
     <t>Australian Gouldian</t>
   </si>
   <si>
@@ -261,6 +258,15 @@
   </si>
   <si>
     <t>Pastel</t>
+  </si>
+  <si>
+    <t>a11</t>
+  </si>
+  <si>
+    <t>a12</t>
+  </si>
+  <si>
+    <t>a13</t>
   </si>
 </sst>
 </file>
@@ -627,10 +633,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" t="s">
         <v>39</v>
-      </c>
-      <c r="B4" t="s">
-        <v>40</v>
       </c>
       <c r="C4">
         <v>111</v>
@@ -638,10 +644,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" t="s">
         <v>41</v>
-      </c>
-      <c r="B5" t="s">
-        <v>42</v>
       </c>
       <c r="C5">
         <v>1121</v>
@@ -649,10 +655,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C6">
         <v>2</v>
@@ -660,10 +666,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" t="s">
         <v>44</v>
-      </c>
-      <c r="B7" t="s">
-        <v>45</v>
       </c>
       <c r="C7">
         <v>334</v>
@@ -671,10 +677,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" t="s">
         <v>46</v>
-      </c>
-      <c r="B8" t="s">
-        <v>47</v>
       </c>
       <c r="C8">
         <v>106</v>
@@ -682,10 +688,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" t="s">
         <v>49</v>
-      </c>
-      <c r="B9" t="s">
-        <v>50</v>
       </c>
       <c r="C9">
         <v>102</v>
@@ -693,10 +699,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" t="s">
         <v>52</v>
-      </c>
-      <c r="B10" t="s">
-        <v>53</v>
       </c>
       <c r="C10">
         <v>1113</v>
@@ -704,10 +710,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11" t="s">
         <v>55</v>
-      </c>
-      <c r="B11" t="s">
-        <v>56</v>
       </c>
       <c r="C11">
         <v>121</v>
@@ -715,10 +721,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" t="s">
         <v>57</v>
-      </c>
-      <c r="B12" t="s">
-        <v>58</v>
       </c>
       <c r="C12">
         <v>999</v>
@@ -726,10 +732,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>58</v>
+      </c>
+      <c r="B13" t="s">
         <v>59</v>
-      </c>
-      <c r="B13" t="s">
-        <v>60</v>
       </c>
       <c r="C13">
         <v>333</v>
@@ -737,10 +743,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>60</v>
+      </c>
+      <c r="B14" t="s">
         <v>61</v>
-      </c>
-      <c r="B14" t="s">
-        <v>62</v>
       </c>
       <c r="C14">
         <v>555</v>
@@ -748,10 +754,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>62</v>
+      </c>
+      <c r="B15" t="s">
         <v>63</v>
-      </c>
-      <c r="B15" t="s">
-        <v>64</v>
       </c>
       <c r="C15">
         <v>777</v>
@@ -759,10 +765,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>70</v>
+      </c>
+      <c r="B16" t="s">
         <v>71</v>
-      </c>
-      <c r="B16" t="s">
-        <v>72</v>
       </c>
       <c r="C16">
         <v>757575</v>
@@ -778,7 +784,7 @@
   <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -823,13 +829,13 @@
         <v>14</v>
       </c>
       <c r="J1" t="s">
+        <v>67</v>
+      </c>
+      <c r="K1" t="s">
         <v>68</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>69</v>
-      </c>
-      <c r="L1" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
@@ -849,19 +855,19 @@
         <v>45048</v>
       </c>
       <c r="H2" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="I2">
         <v>1</v>
       </c>
       <c r="J2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K2" t="s">
+        <v>65</v>
+      </c>
+      <c r="L2" t="s">
         <v>66</v>
-      </c>
-      <c r="L2" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
@@ -869,10 +875,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" t="s">
         <v>33</v>
-      </c>
-      <c r="C3" t="s">
-        <v>34</v>
       </c>
       <c r="D3" t="s">
         <v>31</v>
@@ -881,19 +887,19 @@
         <v>45048</v>
       </c>
       <c r="H3" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="I3">
         <v>1</v>
       </c>
       <c r="J3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K3" t="s">
+        <v>65</v>
+      </c>
+      <c r="L3" t="s">
         <v>66</v>
-      </c>
-      <c r="L3" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
@@ -901,31 +907,31 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" t="s">
         <v>35</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>36</v>
-      </c>
-      <c r="D4" t="s">
-        <v>37</v>
       </c>
       <c r="G4" s="1">
         <v>45048</v>
       </c>
       <c r="H4" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="I4">
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K4" t="s">
+        <v>65</v>
+      </c>
+      <c r="L4" t="s">
         <v>66</v>
-      </c>
-      <c r="L4" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
@@ -933,10 +939,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D5" t="s">
         <v>31</v>
@@ -951,13 +957,13 @@
         <v>1</v>
       </c>
       <c r="J5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K5" t="s">
+        <v>65</v>
+      </c>
+      <c r="L5" t="s">
         <v>66</v>
-      </c>
-      <c r="L5" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
@@ -971,7 +977,7 @@
         <v>30</v>
       </c>
       <c r="D6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G6" s="1">
         <v>45048</v>
@@ -983,13 +989,13 @@
         <v>1</v>
       </c>
       <c r="J6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K6" t="s">
+        <v>65</v>
+      </c>
+      <c r="L6" t="s">
         <v>66</v>
-      </c>
-      <c r="L6" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
@@ -997,31 +1003,31 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" t="s">
         <v>35</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>36</v>
-      </c>
-      <c r="D7" t="s">
-        <v>37</v>
       </c>
       <c r="G7" s="1">
         <v>45049</v>
       </c>
       <c r="H7" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="I7">
         <v>106</v>
       </c>
       <c r="J7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K7" t="s">
+        <v>65</v>
+      </c>
+      <c r="L7" t="s">
         <v>66</v>
-      </c>
-      <c r="L7" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
@@ -1041,19 +1047,19 @@
         <v>45049</v>
       </c>
       <c r="H8" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="I8">
         <v>102</v>
       </c>
       <c r="J8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K8" t="s">
+        <v>65</v>
+      </c>
+      <c r="L8" t="s">
         <v>66</v>
-      </c>
-      <c r="L8" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
@@ -1061,13 +1067,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G9" s="1">
         <v>45049</v>
@@ -1079,13 +1085,13 @@
         <v>1</v>
       </c>
       <c r="J9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K9" t="s">
+        <v>65</v>
+      </c>
+      <c r="L9" t="s">
         <v>66</v>
-      </c>
-      <c r="L9" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
@@ -1093,10 +1099,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" t="s">
         <v>35</v>
-      </c>
-      <c r="C10" t="s">
-        <v>36</v>
       </c>
       <c r="D10" t="s">
         <v>31</v>
@@ -1111,19 +1117,19 @@
         <v>45049</v>
       </c>
       <c r="H10" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="I10">
         <v>1</v>
       </c>
       <c r="J10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K10" t="s">
+        <v>65</v>
+      </c>
+      <c r="L10" t="s">
         <v>66</v>
-      </c>
-      <c r="L10" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
@@ -1155,13 +1161,13 @@
         <v>1</v>
       </c>
       <c r="J11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K11" t="s">
+        <v>65</v>
+      </c>
+      <c r="L11" t="s">
         <v>66</v>
-      </c>
-      <c r="L11" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
@@ -1175,7 +1181,7 @@
         <v>30</v>
       </c>
       <c r="D12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E12">
         <v>10</v>
@@ -1190,13 +1196,13 @@
         <v>1</v>
       </c>
       <c r="J12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K12" t="s">
+        <v>65</v>
+      </c>
+      <c r="L12" t="s">
         <v>66</v>
-      </c>
-      <c r="L12" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
@@ -1204,13 +1210,13 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G13" s="1">
         <v>45050</v>
@@ -1222,13 +1228,13 @@
         <v>777</v>
       </c>
       <c r="J13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K13" t="s">
+        <v>65</v>
+      </c>
+      <c r="L13" t="s">
         <v>66</v>
-      </c>
-      <c r="L13" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
@@ -1236,13 +1242,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E14">
         <v>7</v>
@@ -1260,13 +1266,13 @@
         <v>777</v>
       </c>
       <c r="J14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K14" t="s">
+        <v>65</v>
+      </c>
+      <c r="L14" t="s">
         <v>66</v>
-      </c>
-      <c r="L14" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
@@ -1274,13 +1280,13 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" t="s">
         <v>35</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>36</v>
-      </c>
-      <c r="D15" t="s">
-        <v>37</v>
       </c>
       <c r="G15" s="1">
         <v>45054</v>
@@ -1292,13 +1298,13 @@
         <v>777</v>
       </c>
       <c r="J15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K15" t="s">
+        <v>65</v>
+      </c>
+      <c r="L15" t="s">
         <v>66</v>
-      </c>
-      <c r="L15" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
@@ -1312,25 +1318,25 @@
         <v>30</v>
       </c>
       <c r="D16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G16" s="1">
         <v>45055</v>
       </c>
       <c r="H16" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="I16">
         <v>757575</v>
       </c>
       <c r="J16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K16" t="s">
+        <v>65</v>
+      </c>
+      <c r="L16" t="s">
         <v>66</v>
-      </c>
-      <c r="L16" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
@@ -1338,10 +1344,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" t="s">
         <v>35</v>
-      </c>
-      <c r="C17" t="s">
-        <v>36</v>
       </c>
       <c r="D17" t="s">
         <v>31</v>
@@ -1356,13 +1362,13 @@
         <v>757575</v>
       </c>
       <c r="J17" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K17" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L17" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
@@ -1370,13 +1376,13 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" t="s">
         <v>35</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>36</v>
-      </c>
-      <c r="D18" t="s">
-        <v>37</v>
       </c>
       <c r="G18" s="1">
         <v>45055</v>
@@ -1388,13 +1394,13 @@
         <v>757575</v>
       </c>
       <c r="J18" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
@@ -1402,13 +1408,13 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" t="s">
         <v>35</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>36</v>
-      </c>
-      <c r="D19" t="s">
-        <v>37</v>
       </c>
       <c r="G19" s="1">
         <v>45055</v>
@@ -1420,13 +1426,13 @@
         <v>757575</v>
       </c>
       <c r="J19" t="s">
+        <v>74</v>
+      </c>
+      <c r="K19" t="s">
+        <v>65</v>
+      </c>
+      <c r="L19" t="s">
         <v>75</v>
-      </c>
-      <c r="K19" t="s">
-        <v>66</v>
-      </c>
-      <c r="L19" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
@@ -1434,10 +1440,10 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" t="s">
         <v>35</v>
-      </c>
-      <c r="C20" t="s">
-        <v>36</v>
       </c>
       <c r="D20" t="s">
         <v>31</v>
@@ -1458,13 +1464,13 @@
         <v>757575</v>
       </c>
       <c r="J20" t="s">
+        <v>74</v>
+      </c>
+      <c r="K20" t="s">
+        <v>65</v>
+      </c>
+      <c r="L20" t="s">
         <v>75</v>
-      </c>
-      <c r="K20" t="s">
-        <v>66</v>
-      </c>
-      <c r="L20" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
@@ -1472,13 +1478,13 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" t="s">
         <v>35</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>36</v>
-      </c>
-      <c r="D21" t="s">
-        <v>37</v>
       </c>
       <c r="E21">
         <v>16</v>
@@ -1496,13 +1502,13 @@
         <v>757575</v>
       </c>
       <c r="J21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L21" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -1512,7 +1518,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38953711-B99E-424A-A94F-86EB399A85F5}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -1658,7 +1664,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B9">
         <v>6</v>
@@ -1675,7 +1681,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -1687,6 +1693,57 @@
         <v>9</v>
       </c>
       <c r="E10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>77</v>
+      </c>
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11">
+        <v>3</v>
+      </c>
+      <c r="D11">
+        <v>3</v>
+      </c>
+      <c r="E11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>78</v>
+      </c>
+      <c r="B12">
+        <v>-4</v>
+      </c>
+      <c r="C12">
+        <v>-5</v>
+      </c>
+      <c r="D12">
+        <v>-6</v>
+      </c>
+      <c r="E12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>79</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="E13" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added edit cage and bird
</commit_message>
<xml_diff>
--- a/LoginPage/bin/Debug/net7.0-windows/Data/birds.xlsx
+++ b/LoginPage/bin/Debug/net7.0-windows/Data/birds.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aviv1\Desktop\Bird-Project-For-College\LoginPage\bin\Debug\net7.0-windows\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tomer\source\repos\Bird-Project-For-College\LoginPage\bin\Debug\net7.0-windows\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FBA11BD-DBF7-446F-BF6E-8BAEB9C116F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5ABD04E-9016-49F4-8FDA-4DF69345C118}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11295" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="89">
   <si>
     <t>bdika11</t>
   </si>
@@ -155,9 +155,6 @@
     <t>Tomer9!!</t>
   </si>
   <si>
-    <t>ש</t>
-  </si>
-  <si>
     <t>kakape98</t>
   </si>
   <si>
@@ -279,6 +276,24 @@
   </si>
   <si>
     <t>a15</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>a16</t>
+  </si>
+  <si>
+    <t>a17</t>
+  </si>
+  <si>
+    <t>a18</t>
+  </si>
+  <si>
+    <t>a19</t>
+  </si>
+  <si>
+    <t>a20</t>
   </si>
 </sst>
 </file>
@@ -600,7 +615,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -667,10 +682,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>83</v>
       </c>
       <c r="B6" t="s">
-        <v>42</v>
+        <v>83</v>
       </c>
       <c r="C6">
         <v>2</v>
@@ -678,10 +693,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" t="s">
         <v>43</v>
-      </c>
-      <c r="B7" t="s">
-        <v>44</v>
       </c>
       <c r="C7">
         <v>334</v>
@@ -689,10 +704,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" t="s">
         <v>45</v>
-      </c>
-      <c r="B8" t="s">
-        <v>46</v>
       </c>
       <c r="C8">
         <v>106</v>
@@ -700,10 +715,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" t="s">
         <v>48</v>
-      </c>
-      <c r="B9" t="s">
-        <v>49</v>
       </c>
       <c r="C9">
         <v>102</v>
@@ -711,10 +726,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" t="s">
         <v>51</v>
-      </c>
-      <c r="B10" t="s">
-        <v>52</v>
       </c>
       <c r="C10">
         <v>1113</v>
@@ -722,10 +737,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" t="s">
         <v>54</v>
-      </c>
-      <c r="B11" t="s">
-        <v>55</v>
       </c>
       <c r="C11">
         <v>121</v>
@@ -733,10 +748,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>55</v>
+      </c>
+      <c r="B12" t="s">
         <v>56</v>
-      </c>
-      <c r="B12" t="s">
-        <v>57</v>
       </c>
       <c r="C12">
         <v>999</v>
@@ -744,10 +759,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13" t="s">
         <v>58</v>
-      </c>
-      <c r="B13" t="s">
-        <v>59</v>
       </c>
       <c r="C13">
         <v>333</v>
@@ -755,10 +770,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14" t="s">
         <v>60</v>
-      </c>
-      <c r="B14" t="s">
-        <v>61</v>
       </c>
       <c r="C14">
         <v>555</v>
@@ -766,10 +781,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>61</v>
+      </c>
+      <c r="B15" t="s">
         <v>62</v>
-      </c>
-      <c r="B15" t="s">
-        <v>63</v>
       </c>
       <c r="C15">
         <v>777</v>
@@ -777,10 +792,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>69</v>
+      </c>
+      <c r="B16" t="s">
         <v>70</v>
-      </c>
-      <c r="B16" t="s">
-        <v>71</v>
       </c>
       <c r="C16">
         <v>757575</v>
@@ -793,10 +808,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54D0F034-6ABF-4A1B-831B-4EE238759774}">
-  <dimension ref="A1:L24"/>
+  <dimension ref="A1:L34"/>
   <sheetViews>
-    <sheetView rightToLeft="1" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -841,13 +856,13 @@
         <v>14</v>
       </c>
       <c r="J1" t="s">
+        <v>66</v>
+      </c>
+      <c r="K1" t="s">
         <v>67</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>68</v>
-      </c>
-      <c r="L1" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
@@ -873,13 +888,13 @@
         <v>1</v>
       </c>
       <c r="J2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
@@ -905,13 +920,13 @@
         <v>1</v>
       </c>
       <c r="J3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
@@ -931,19 +946,19 @@
         <v>45048</v>
       </c>
       <c r="H4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="I4">
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
@@ -969,13 +984,13 @@
         <v>1</v>
       </c>
       <c r="J5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
@@ -1001,13 +1016,13 @@
         <v>1</v>
       </c>
       <c r="J6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
@@ -1033,13 +1048,13 @@
         <v>1</v>
       </c>
       <c r="J7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
@@ -1065,13 +1080,13 @@
         <v>1</v>
       </c>
       <c r="J8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
@@ -1082,7 +1097,7 @@
         <v>34</v>
       </c>
       <c r="C9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D9" t="s">
         <v>36</v>
@@ -1097,13 +1112,13 @@
         <v>1</v>
       </c>
       <c r="J9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
@@ -1135,13 +1150,13 @@
         <v>1</v>
       </c>
       <c r="J10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
@@ -1173,13 +1188,13 @@
         <v>1</v>
       </c>
       <c r="J11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
@@ -1208,13 +1223,13 @@
         <v>1</v>
       </c>
       <c r="J12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
@@ -1225,7 +1240,7 @@
         <v>34</v>
       </c>
       <c r="C13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D13" t="s">
         <v>36</v>
@@ -1240,13 +1255,13 @@
         <v>1</v>
       </c>
       <c r="J13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
@@ -1257,7 +1272,7 @@
         <v>34</v>
       </c>
       <c r="C14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D14" t="s">
         <v>36</v>
@@ -1278,13 +1293,13 @@
         <v>1</v>
       </c>
       <c r="J14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
@@ -1310,13 +1325,13 @@
         <v>1</v>
       </c>
       <c r="J15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
@@ -1342,13 +1357,13 @@
         <v>1</v>
       </c>
       <c r="J16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
@@ -1374,13 +1389,13 @@
         <v>1</v>
       </c>
       <c r="J17" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K17" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
@@ -1406,13 +1421,13 @@
         <v>1</v>
       </c>
       <c r="J18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K18" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
@@ -1438,13 +1453,13 @@
         <v>1</v>
       </c>
       <c r="J19" t="s">
+        <v>73</v>
+      </c>
+      <c r="K19" t="s">
+        <v>64</v>
+      </c>
+      <c r="L19" t="s">
         <v>74</v>
-      </c>
-      <c r="K19" t="s">
-        <v>65</v>
-      </c>
-      <c r="L19" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
@@ -1476,13 +1491,13 @@
         <v>1</v>
       </c>
       <c r="J20" t="s">
+        <v>73</v>
+      </c>
+      <c r="K20" t="s">
+        <v>64</v>
+      </c>
+      <c r="L20" t="s">
         <v>74</v>
-      </c>
-      <c r="K20" t="s">
-        <v>65</v>
-      </c>
-      <c r="L20" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
@@ -1514,13 +1529,13 @@
         <v>1</v>
       </c>
       <c r="J21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L21" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
@@ -1531,7 +1546,7 @@
         <v>29</v>
       </c>
       <c r="C22" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D22" t="s">
         <v>36</v>
@@ -1540,19 +1555,19 @@
         <v>45062</v>
       </c>
       <c r="H22" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I22">
         <v>757575</v>
       </c>
       <c r="J22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K22" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L22" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
@@ -1572,19 +1587,19 @@
         <v>45062</v>
       </c>
       <c r="H23" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I23">
         <v>757575</v>
       </c>
       <c r="J23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K23" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L23" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
@@ -1595,7 +1610,7 @@
         <v>29</v>
       </c>
       <c r="C24" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D24" t="s">
         <v>36</v>
@@ -1607,19 +1622,360 @@
         <v>45062</v>
       </c>
       <c r="H24" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I24">
         <v>757575</v>
       </c>
       <c r="J24" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L24" t="s">
-        <v>66</v>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>34</v>
+      </c>
+      <c r="C25" t="s">
+        <v>35</v>
+      </c>
+      <c r="D25" t="s">
+        <v>36</v>
+      </c>
+      <c r="G25" s="1">
+        <v>45065</v>
+      </c>
+      <c r="H25" t="s">
+        <v>82</v>
+      </c>
+      <c r="I25">
+        <v>2</v>
+      </c>
+      <c r="J25" t="s">
+        <v>63</v>
+      </c>
+      <c r="K25" t="s">
+        <v>64</v>
+      </c>
+      <c r="L25" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>34</v>
+      </c>
+      <c r="C26" t="s">
+        <v>35</v>
+      </c>
+      <c r="D26" t="s">
+        <v>36</v>
+      </c>
+      <c r="E26">
+        <v>2</v>
+      </c>
+      <c r="F26">
+        <v>3</v>
+      </c>
+      <c r="G26" s="1">
+        <v>45065</v>
+      </c>
+      <c r="H26" t="s">
+        <v>86</v>
+      </c>
+      <c r="I26">
+        <v>2</v>
+      </c>
+      <c r="J26" t="s">
+        <v>63</v>
+      </c>
+      <c r="K26" t="s">
+        <v>64</v>
+      </c>
+      <c r="L26" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27" t="s">
+        <v>52</v>
+      </c>
+      <c r="D27" t="s">
+        <v>36</v>
+      </c>
+      <c r="F27">
+        <v>5</v>
+      </c>
+      <c r="G27" s="1">
+        <v>45065</v>
+      </c>
+      <c r="H27" t="s">
+        <v>82</v>
+      </c>
+      <c r="I27">
+        <v>2</v>
+      </c>
+      <c r="J27" t="s">
+        <v>73</v>
+      </c>
+      <c r="K27" t="s">
+        <v>64</v>
+      </c>
+      <c r="L27" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>32</v>
+      </c>
+      <c r="C28" t="s">
+        <v>33</v>
+      </c>
+      <c r="D28" t="s">
+        <v>36</v>
+      </c>
+      <c r="G28" s="1">
+        <v>45065</v>
+      </c>
+      <c r="H28" t="s">
+        <v>82</v>
+      </c>
+      <c r="I28">
+        <v>2</v>
+      </c>
+      <c r="J28" t="s">
+        <v>63</v>
+      </c>
+      <c r="K28" t="s">
+        <v>64</v>
+      </c>
+      <c r="L28" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>29</v>
+      </c>
+      <c r="C29" t="s">
+        <v>30</v>
+      </c>
+      <c r="D29" t="s">
+        <v>31</v>
+      </c>
+      <c r="G29" s="1">
+        <v>45065</v>
+      </c>
+      <c r="H29" t="s">
+        <v>82</v>
+      </c>
+      <c r="I29">
+        <v>2</v>
+      </c>
+      <c r="J29" t="s">
+        <v>73</v>
+      </c>
+      <c r="K29" t="s">
+        <v>64</v>
+      </c>
+      <c r="L29" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>34</v>
+      </c>
+      <c r="C30" t="s">
+        <v>35</v>
+      </c>
+      <c r="D30" t="s">
+        <v>31</v>
+      </c>
+      <c r="G30" s="1">
+        <v>45065</v>
+      </c>
+      <c r="H30" t="s">
+        <v>19</v>
+      </c>
+      <c r="I30">
+        <v>1</v>
+      </c>
+      <c r="J30" t="s">
+        <v>63</v>
+      </c>
+      <c r="K30" t="s">
+        <v>64</v>
+      </c>
+      <c r="L30" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>34</v>
+      </c>
+      <c r="C31" t="s">
+        <v>35</v>
+      </c>
+      <c r="D31" t="s">
+        <v>31</v>
+      </c>
+      <c r="G31" s="1">
+        <v>45065</v>
+      </c>
+      <c r="H31" t="s">
+        <v>19</v>
+      </c>
+      <c r="I31">
+        <v>1</v>
+      </c>
+      <c r="J31" t="s">
+        <v>63</v>
+      </c>
+      <c r="K31" t="s">
+        <v>64</v>
+      </c>
+      <c r="L31" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>29</v>
+      </c>
+      <c r="C32" t="s">
+        <v>30</v>
+      </c>
+      <c r="D32" t="s">
+        <v>36</v>
+      </c>
+      <c r="G32" s="1">
+        <v>45065</v>
+      </c>
+      <c r="H32" t="s">
+        <v>19</v>
+      </c>
+      <c r="I32">
+        <v>1</v>
+      </c>
+      <c r="J32" t="s">
+        <v>73</v>
+      </c>
+      <c r="K32" t="s">
+        <v>64</v>
+      </c>
+      <c r="L32" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>34</v>
+      </c>
+      <c r="C33" t="s">
+        <v>35</v>
+      </c>
+      <c r="D33" t="s">
+        <v>36</v>
+      </c>
+      <c r="E33">
+        <v>2</v>
+      </c>
+      <c r="F33">
+        <v>3</v>
+      </c>
+      <c r="G33" s="1">
+        <v>45065</v>
+      </c>
+      <c r="H33" t="s">
+        <v>21</v>
+      </c>
+      <c r="I33">
+        <v>1</v>
+      </c>
+      <c r="J33" t="s">
+        <v>63</v>
+      </c>
+      <c r="K33" t="s">
+        <v>64</v>
+      </c>
+      <c r="L33" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>34</v>
+      </c>
+      <c r="C34" t="s">
+        <v>35</v>
+      </c>
+      <c r="D34" t="s">
+        <v>36</v>
+      </c>
+      <c r="E34">
+        <v>2</v>
+      </c>
+      <c r="F34">
+        <v>3</v>
+      </c>
+      <c r="G34" s="1">
+        <v>45065</v>
+      </c>
+      <c r="H34" t="s">
+        <v>21</v>
+      </c>
+      <c r="I34">
+        <v>1</v>
+      </c>
+      <c r="J34" t="s">
+        <v>63</v>
+      </c>
+      <c r="K34" t="s">
+        <v>64</v>
+      </c>
+      <c r="L34" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1629,10 +1985,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38953711-B99E-424A-A94F-86EB399A85F5}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView rightToLeft="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1660,7 +2016,7 @@
         <v>18</v>
       </c>
       <c r="F1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -1668,16 +2024,16 @@
         <v>19</v>
       </c>
       <c r="B2">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="C2">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="D2">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="E2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -1708,16 +2064,16 @@
         <v>23</v>
       </c>
       <c r="B4">
+        <v>44</v>
+      </c>
+      <c r="C4">
+        <v>44</v>
+      </c>
+      <c r="D4">
+        <v>44</v>
+      </c>
+      <c r="E4" t="s">
         <v>22</v>
-      </c>
-      <c r="C4">
-        <v>222</v>
-      </c>
-      <c r="D4">
-        <v>22</v>
-      </c>
-      <c r="E4" t="s">
-        <v>20</v>
       </c>
       <c r="F4">
         <v>1</v>
@@ -1760,7 +2116,7 @@
         <v>22</v>
       </c>
       <c r="F6">
-        <v>111</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -1780,7 +2136,7 @@
         <v>27</v>
       </c>
       <c r="F7">
-        <v>111</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -1800,12 +2156,12 @@
         <v>20</v>
       </c>
       <c r="F8">
-        <v>111</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B9">
         <v>6</v>
@@ -1820,12 +2176,12 @@
         <v>20</v>
       </c>
       <c r="F9">
-        <v>111</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -1840,12 +2196,12 @@
         <v>20</v>
       </c>
       <c r="F10">
-        <v>111</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B11">
         <v>3</v>
@@ -1860,12 +2216,12 @@
         <v>22</v>
       </c>
       <c r="F11">
-        <v>111</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B12">
         <v>-4</v>
@@ -1880,12 +2236,12 @@
         <v>20</v>
       </c>
       <c r="F12">
-        <v>111</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B13">
         <v>2</v>
@@ -1900,12 +2256,12 @@
         <v>20</v>
       </c>
       <c r="F13">
-        <v>111</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -1920,12 +2276,12 @@
         <v>20</v>
       </c>
       <c r="F14">
-        <v>757575</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B15">
         <v>12</v>
@@ -1940,7 +2296,107 @@
         <v>27</v>
       </c>
       <c r="F15">
-        <v>757575</v>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>84</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16">
+        <v>4</v>
+      </c>
+      <c r="D16">
+        <v>5</v>
+      </c>
+      <c r="E16" t="s">
+        <v>20</v>
+      </c>
+      <c r="F16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>85</v>
+      </c>
+      <c r="B17">
+        <v>5</v>
+      </c>
+      <c r="C17">
+        <v>5</v>
+      </c>
+      <c r="D17">
+        <v>5</v>
+      </c>
+      <c r="E17" t="s">
+        <v>22</v>
+      </c>
+      <c r="F17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>86</v>
+      </c>
+      <c r="B18">
+        <v>5</v>
+      </c>
+      <c r="C18">
+        <v>3</v>
+      </c>
+      <c r="D18">
+        <v>2</v>
+      </c>
+      <c r="E18" t="s">
+        <v>20</v>
+      </c>
+      <c r="F18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>87</v>
+      </c>
+      <c r="B19">
+        <v>32</v>
+      </c>
+      <c r="C19">
+        <v>23</v>
+      </c>
+      <c r="D19">
+        <v>234</v>
+      </c>
+      <c r="E19" t="s">
+        <v>20</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>88</v>
+      </c>
+      <c r="B20">
+        <v>66</v>
+      </c>
+      <c r="C20">
+        <v>66</v>
+      </c>
+      <c r="D20">
+        <v>66</v>
+      </c>
+      <c r="E20" t="s">
+        <v>20</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finel for real this time
</commit_message>
<xml_diff>
--- a/LoginPage/bin/Debug/net7.0-windows/Data/birds.xlsx
+++ b/LoginPage/bin/Debug/net7.0-windows/Data/birds.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aviv1\source\repos\Bird-Project-For-College\LoginPage\bin\Debug\net7.0-windows\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tomer\Documents\Tomer\SCE\2nd-year\2-semester\QA course\BirdsProject\LoginPage\bin\Debug\net7.0-windows\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B3E192B-E79A-4A91-9DD8-586D85B74891}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C1922BB-11BC-4BDA-9800-263C1E9B3A6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11295" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11295" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="133">
   <si>
     <t>bdika11</t>
   </si>
@@ -417,6 +417,15 @@
   </si>
   <si>
     <t>White</t>
+  </si>
+  <si>
+    <t>arvili75</t>
+  </si>
+  <si>
+    <t>a42</t>
+  </si>
+  <si>
+    <t>a43</t>
   </si>
 </sst>
 </file>
@@ -735,7 +744,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C33"/>
+  <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
@@ -1111,6 +1120,17 @@
         <v>8033</v>
       </c>
     </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>130</v>
+      </c>
+      <c r="B34" t="s">
+        <v>71</v>
+      </c>
+      <c r="C34">
+        <v>8034</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1118,7 +1138,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54D0F034-6ABF-4A1B-831B-4EE238759774}">
-  <dimension ref="A1:L53"/>
+  <dimension ref="A1:L56"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="I23" sqref="I23"/>
@@ -2935,6 +2955,108 @@
         <v>66</v>
       </c>
     </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>34</v>
+      </c>
+      <c r="C54" t="s">
+        <v>35</v>
+      </c>
+      <c r="D54" t="s">
+        <v>36</v>
+      </c>
+      <c r="G54" s="1">
+        <v>45077</v>
+      </c>
+      <c r="H54" t="s">
+        <v>132</v>
+      </c>
+      <c r="I54">
+        <v>8034</v>
+      </c>
+      <c r="J54" t="s">
+        <v>64</v>
+      </c>
+      <c r="K54" t="s">
+        <v>65</v>
+      </c>
+      <c r="L54" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>34</v>
+      </c>
+      <c r="C55" t="s">
+        <v>35</v>
+      </c>
+      <c r="D55" t="s">
+        <v>31</v>
+      </c>
+      <c r="G55" s="1">
+        <v>45077</v>
+      </c>
+      <c r="H55" t="s">
+        <v>131</v>
+      </c>
+      <c r="I55">
+        <v>8034</v>
+      </c>
+      <c r="J55" t="s">
+        <v>64</v>
+      </c>
+      <c r="K55" t="s">
+        <v>65</v>
+      </c>
+      <c r="L55" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>34</v>
+      </c>
+      <c r="C56" t="s">
+        <v>35</v>
+      </c>
+      <c r="D56" t="s">
+        <v>36</v>
+      </c>
+      <c r="E56">
+        <v>54</v>
+      </c>
+      <c r="F56">
+        <v>53</v>
+      </c>
+      <c r="G56" s="1">
+        <v>45077</v>
+      </c>
+      <c r="H56" t="s">
+        <v>131</v>
+      </c>
+      <c r="I56">
+        <v>8034</v>
+      </c>
+      <c r="J56" t="s">
+        <v>64</v>
+      </c>
+      <c r="K56" t="s">
+        <v>65</v>
+      </c>
+      <c r="L56" t="s">
+        <v>66</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2942,7 +3064,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38953711-B99E-424A-A94F-86EB399A85F5}">
-  <dimension ref="A1:F41"/>
+  <dimension ref="A1:F43"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
@@ -3776,6 +3898,46 @@
         <v>8033</v>
       </c>
     </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>131</v>
+      </c>
+      <c r="B42">
+        <v>2</v>
+      </c>
+      <c r="C42">
+        <v>2</v>
+      </c>
+      <c r="D42">
+        <v>144</v>
+      </c>
+      <c r="E42" t="s">
+        <v>20</v>
+      </c>
+      <c r="F42">
+        <v>8034</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>132</v>
+      </c>
+      <c r="B43">
+        <v>2</v>
+      </c>
+      <c r="C43">
+        <v>4</v>
+      </c>
+      <c r="D43">
+        <v>5</v>
+      </c>
+      <c r="E43" t="s">
+        <v>20</v>
+      </c>
+      <c r="F43">
+        <v>8034</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>